<commit_message>
update require xls and bmpr
</commit_message>
<xml_diff>
--- a/doc/01_design/require.xlsx
+++ b/doc/01_design/require.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>SCW图片管理</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,18 +35,6 @@
   </si>
   <si>
     <t>1.主要功能: 每个账号都能上传、下载、删除若干图片。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二、 管理员: 设有若干个管理员, 该管理员能管理每个账号上传的图片。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.主要功能: 为每个账号上传的照片标记通过、打回状态, 填写打回理由。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.次要功能: 能查看所有管理员的管理操作日志。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -60,6 +48,22 @@
   <si>
     <t xml:space="preserve"> V0.2 2015-10-8
 POWERED BY SCW TEAM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二、 管理员: 设有若干个管理员, 该管理员能管理每个账号上传的图片。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.主要功能①: 为每个账号上传的照片标记通过、打回状态, 填写打回理由。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.主要功能②: 为每个账号添加问题图片。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.次要功能: 能查看所有管理员的管理操作日志。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -122,8 +126,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -148,17 +162,27 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,7 +515,7 @@
   <dimension ref="B8:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -845,7 +869,7 @@
     </row>
     <row r="34" spans="2:14">
       <c r="B34" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -907,10 +931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -932,27 +956,32 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>